<commit_message>
add bars on each farms, upgraded labels on values, correct bugs on reversion, add summaries on the end of day 7
</commit_message>
<xml_diff>
--- a/Assets/Data/Dataset.xlsx
+++ b/Assets/Data/Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_learning\Immersive-Water-Quality-main-t2\Immersive-Water-Quality-main\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F52ABF3-6878-4B63-9A9F-49FD567C7261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8D07F6-E052-482A-AD13-B07193C91875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19298" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,13 +191,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -207,7 +208,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL22"/>
+  <dimension ref="A1:AL29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -500,43 +501,44 @@
     <col min="2" max="2" width="16.125" customWidth="1"/>
     <col min="3" max="3" width="30.375" customWidth="1"/>
     <col min="4" max="5" width="33.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="6" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -608,10 +610,10 @@
       <c r="X2" t="s">
         <v>15</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="Y2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="Z2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="AA2" t="s">
@@ -1531,884 +1533,1738 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>44906</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="C13" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.88387499999999997</v>
-      </c>
-      <c r="F13" s="2">
-        <v>44906</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.27316741751617901</v>
-      </c>
-      <c r="H13" s="3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>44856</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1.076875</v>
+      </c>
+      <c r="F13" s="8">
+        <v>44856</v>
+      </c>
+      <c r="G13">
+        <v>0.66995425417614596</v>
+      </c>
+      <c r="H13">
         <f t="shared" ref="H13:H19" si="12">EXP(0.44*LN(G13)-0.77)</f>
-        <v>0.26159049735751211</v>
-      </c>
-      <c r="I13" s="3">
+        <v>0.38819784001667268</v>
+      </c>
+      <c r="I13">
         <f t="shared" ref="I13:I19" si="13">H13*G13</f>
-        <v>7.1458000609924438E-2</v>
-      </c>
-      <c r="J13" s="3">
-        <v>23.6090931392675</v>
-      </c>
-      <c r="K13" s="3">
-        <v>0.67524408493948995</v>
-      </c>
-      <c r="L13" s="3">
+        <v>0.26007479438116077</v>
+      </c>
+      <c r="J13">
+        <v>51.601810700027102</v>
+      </c>
+      <c r="K13">
+        <v>1.6560637114991801</v>
+      </c>
+      <c r="L13">
         <v>5</v>
       </c>
-      <c r="M13" s="3">
-        <v>0</v>
-      </c>
-      <c r="N13" s="3">
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
         <f t="shared" ref="N13:N19" si="14">IF(M13=0,0,EXP(0.44*LN(M13)-0.77))</f>
         <v>0</v>
       </c>
-      <c r="O13" s="3" t="str">
+      <c r="O13" t="str">
         <f t="shared" ref="O13:O19" si="15">IF(M13=0,"NA",N13*M13)</f>
         <v>NA</v>
       </c>
-      <c r="P13" s="3">
-        <v>0.27316741751617901</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>44906</v>
-      </c>
-      <c r="R13" s="3">
-        <v>0.27316741751617901</v>
-      </c>
-      <c r="S13" s="3">
+      <c r="P13">
+        <v>0.66995425417614596</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>44856</v>
+      </c>
+      <c r="R13">
+        <v>0.66995425417614596</v>
+      </c>
+      <c r="S13">
         <f t="shared" ref="S13:S19" si="16">EXP(0.44*LN(R13)-0.77)</f>
-        <v>0.26159049735751211</v>
-      </c>
-      <c r="T13" s="3">
+        <v>0.38819784001667268</v>
+      </c>
+      <c r="T13">
         <f t="shared" ref="T13:T19" si="17">S13*R13</f>
-        <v>7.1458000609924438E-2</v>
-      </c>
-      <c r="U13" s="3">
-        <v>4.0928947137213703</v>
-      </c>
-      <c r="V13" s="3">
-        <v>0.67524408493948995</v>
-      </c>
-      <c r="W13" s="3">
+        <v>0.26007479438116077</v>
+      </c>
+      <c r="U13">
+        <v>38.941486294296602</v>
+      </c>
+      <c r="V13">
+        <v>1.6560637114991801</v>
+      </c>
+      <c r="W13">
         <v>10</v>
       </c>
-      <c r="X13" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="3" t="str">
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="str">
         <f t="shared" ref="Y13:Y19" si="18">IF(X13=0,"NA",EXP(0.44*LN(X13)-0.77))</f>
         <v>NA</v>
       </c>
-      <c r="Z13" s="3">
+      <c r="Z13">
         <f t="shared" ref="Z13:Z19" si="19">IF(X13=0,0,Y13*X13)</f>
         <v>0</v>
       </c>
-      <c r="AA13" s="3">
-        <v>0.27316741751617901</v>
-      </c>
-      <c r="AB13" s="2">
-        <v>44906</v>
-      </c>
-      <c r="AC13" s="3">
-        <v>0.27316741751617901</v>
-      </c>
-      <c r="AD13" s="3">
+      <c r="AA13">
+        <v>0.66995425417614596</v>
+      </c>
+      <c r="AB13" s="8">
+        <v>44856</v>
+      </c>
+      <c r="AC13">
+        <v>0.66995425417614596</v>
+      </c>
+      <c r="AD13">
         <f t="shared" ref="AD13:AD19" si="20">EXP(0.44*LN(AC13)-0.77)</f>
-        <v>0.26159049735751211</v>
-      </c>
-      <c r="AE13" s="3">
+        <v>0.38819784001667268</v>
+      </c>
+      <c r="AE13">
         <f t="shared" ref="AE13:AE19" si="21">AD13*AC13</f>
-        <v>7.1458000609924438E-2</v>
-      </c>
-      <c r="AF13" s="3">
-        <v>0.83619802381614805</v>
-      </c>
-      <c r="AG13" s="3">
-        <v>0.67524408493948995</v>
-      </c>
-      <c r="AH13" s="3">
-        <v>1.4489930964265301</v>
-      </c>
-      <c r="AI13" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="3" t="str">
+        <v>0.26007479438116077</v>
+      </c>
+      <c r="AF13">
+        <v>1.9400976267077099</v>
+      </c>
+      <c r="AG13">
+        <v>1.6560637114991801</v>
+      </c>
+      <c r="AH13">
+        <v>2.5570327734867901</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13" t="str">
         <f t="shared" ref="AJ13:AJ19" si="22">IF(AI13=0,"NA",EXP(0.44*LN(AI13)-0.77))</f>
         <v>NA</v>
       </c>
-      <c r="AK13" s="3">
+      <c r="AK13">
         <f t="shared" ref="AK13:AK19" si="23">IF(AI13=0,0,AJ13*AI13)</f>
         <v>0</v>
       </c>
-      <c r="AL13" s="3">
-        <v>0.27316741751617901</v>
+      <c r="AL13">
+        <v>0.66995425417614596</v>
       </c>
     </row>
-    <row r="14" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>44907</v>
-      </c>
-      <c r="B14" s="3">
-        <v>18.7</v>
-      </c>
-      <c r="C14" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D14" s="3">
-        <v>1.215125</v>
-      </c>
-      <c r="F14" s="2">
-        <v>44907</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.19642282900661501</v>
-      </c>
-      <c r="H14" s="3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>44857</v>
+      </c>
+      <c r="B14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C14">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D14">
+        <v>1.23875</v>
+      </c>
+      <c r="F14" s="8">
+        <v>44857</v>
+      </c>
+      <c r="G14">
+        <v>0.48173501476434999</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="12"/>
-        <v>0.226254753403314</v>
-      </c>
-      <c r="I14" s="3">
+        <v>0.33575992802457694</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="13"/>
-        <v>4.4441598739672988E-2</v>
-      </c>
-      <c r="J14" s="3">
-        <v>20.905039952458701</v>
-      </c>
-      <c r="K14" s="3">
-        <v>2.2897188533720501</v>
-      </c>
-      <c r="L14" s="3">
+        <v>0.16174731388419666</v>
+      </c>
+      <c r="J14">
+        <v>47.790025582294099</v>
+      </c>
+      <c r="K14">
+        <v>1.19080350865271</v>
+      </c>
+      <c r="L14">
         <v>5</v>
       </c>
-      <c r="M14" s="3">
-        <v>0</v>
-      </c>
-      <c r="N14" s="3">
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="O14" s="3" t="str">
+      <c r="O14" t="str">
         <f t="shared" si="15"/>
         <v>NA</v>
       </c>
-      <c r="P14" s="3">
-        <v>0.19642282900661501</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>44907</v>
-      </c>
-      <c r="R14" s="3">
-        <v>0.19642282900661501</v>
-      </c>
-      <c r="S14" s="3">
+      <c r="P14">
+        <v>0.48173501476434999</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>44857</v>
+      </c>
+      <c r="R14">
+        <v>0.48173501476434999</v>
+      </c>
+      <c r="S14">
         <f t="shared" si="16"/>
-        <v>0.226254753403314</v>
-      </c>
-      <c r="T14" s="3">
+        <v>0.33575992802457694</v>
+      </c>
+      <c r="T14">
         <f t="shared" si="17"/>
-        <v>4.4441598739672988E-2</v>
-      </c>
-      <c r="U14" s="3">
-        <v>2.6998126439276899</v>
-      </c>
-      <c r="V14" s="3">
-        <v>2.2897188533720501</v>
-      </c>
-      <c r="W14" s="3">
-        <v>3.6836052423492398</v>
-      </c>
-      <c r="X14" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="3" t="str">
+        <v>0.16174731388419666</v>
+      </c>
+      <c r="U14">
+        <v>30.130657725655901</v>
+      </c>
+      <c r="V14">
+        <v>1.19080350865271</v>
+      </c>
+      <c r="W14">
+        <v>10</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="str">
         <f t="shared" si="18"/>
         <v>NA</v>
       </c>
-      <c r="Z14" s="3">
+      <c r="Z14">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AA14" s="3">
-        <v>0.19642282900661501</v>
-      </c>
-      <c r="AB14" s="2">
-        <v>44907</v>
-      </c>
-      <c r="AC14" s="3">
-        <v>0.19642282900661501</v>
-      </c>
-      <c r="AD14" s="3">
+      <c r="AA14">
+        <v>0.48173501476434999</v>
+      </c>
+      <c r="AB14" s="8">
+        <v>44857</v>
+      </c>
+      <c r="AC14">
+        <v>0.48173501476434999</v>
+      </c>
+      <c r="AD14">
         <f t="shared" si="20"/>
-        <v>0.226254753403314</v>
-      </c>
-      <c r="AE14" s="3">
+        <v>0.33575992802457694</v>
+      </c>
+      <c r="AE14">
         <f t="shared" si="21"/>
-        <v>4.4441598739672988E-2</v>
-      </c>
-      <c r="AF14" s="3">
-        <v>2.3740459236017402</v>
-      </c>
-      <c r="AG14" s="3">
-        <v>2.2897188533720501</v>
-      </c>
-      <c r="AH14" s="3">
-        <v>0.75257822143453301</v>
-      </c>
-      <c r="AI14" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="3" t="str">
+        <v>0.16174731388419666</v>
+      </c>
+      <c r="AF14">
+        <v>1.38473826466748</v>
+      </c>
+      <c r="AG14">
+        <v>1.19080350865271</v>
+      </c>
+      <c r="AH14">
+        <v>1.7460878640369399</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14" t="str">
         <f t="shared" si="22"/>
         <v>NA</v>
       </c>
-      <c r="AK14" s="3">
+      <c r="AK14">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AL14" s="3">
-        <v>0.19642282900661501</v>
+      <c r="AL14">
+        <v>0.48173501476434999</v>
       </c>
     </row>
-    <row r="15" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>44908</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="C15" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1.206</v>
-      </c>
-      <c r="F15" s="2">
-        <v>44908</v>
-      </c>
-      <c r="G15" s="3">
-        <v>18.183040637561799</v>
-      </c>
-      <c r="H15" s="3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>44858</v>
+      </c>
+      <c r="B15">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C15">
+        <v>2.8</v>
+      </c>
+      <c r="D15">
+        <v>1.34175</v>
+      </c>
+      <c r="F15" s="8">
+        <v>44858</v>
+      </c>
+      <c r="G15">
+        <v>0.346394732182703</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="12"/>
-        <v>1.6590004852178608</v>
-      </c>
-      <c r="I15" s="3">
+        <v>0.29040534914420774</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="13"/>
-        <v>30.165673240451106</v>
-      </c>
-      <c r="J15" s="3">
-        <v>59.657920662264097</v>
-      </c>
-      <c r="K15" s="3">
-        <v>43.756112180507998</v>
-      </c>
-      <c r="L15" s="3">
+        <v>0.1005948831412322</v>
+      </c>
+      <c r="J15">
+        <v>44.511365723431602</v>
+      </c>
+      <c r="K15">
+        <v>1.71494163231468</v>
+      </c>
+      <c r="L15">
         <v>5</v>
       </c>
-      <c r="M15" s="3">
-        <v>0</v>
-      </c>
-      <c r="N15" s="3">
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="O15" s="3" t="str">
+      <c r="O15" t="str">
         <f t="shared" si="15"/>
         <v>NA</v>
       </c>
-      <c r="P15" s="3">
-        <v>18.183040637561799</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>44908</v>
-      </c>
-      <c r="R15" s="3">
-        <v>18.183040637561799</v>
-      </c>
-      <c r="S15" s="3">
+      <c r="P15">
+        <v>0.346394732182703</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>44858</v>
+      </c>
+      <c r="R15">
+        <v>0.346394732182703</v>
+      </c>
+      <c r="S15">
         <f t="shared" si="16"/>
-        <v>1.6590004852178608</v>
-      </c>
-      <c r="T15" s="3">
+        <v>0.29040534914420774</v>
+      </c>
+      <c r="T15">
         <f t="shared" si="17"/>
-        <v>30.165673240451106</v>
-      </c>
-      <c r="U15" s="3">
-        <v>44.023708827339298</v>
-      </c>
-      <c r="V15" s="3">
-        <v>43.756112180507998</v>
-      </c>
-      <c r="W15" s="3">
-        <v>2.42983137953492</v>
-      </c>
-      <c r="X15" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="3" t="str">
+        <v>0.1005948831412322</v>
+      </c>
+      <c r="U15">
+        <v>21.848740114361998</v>
+      </c>
+      <c r="V15">
+        <v>1.71494163231468</v>
+      </c>
+      <c r="W15">
+        <v>10</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="str">
         <f t="shared" si="18"/>
         <v>NA</v>
       </c>
-      <c r="Z15" s="3">
+      <c r="Z15">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AA15" s="3">
-        <v>18.183040637561799</v>
-      </c>
-      <c r="AB15" s="2">
-        <v>44908</v>
-      </c>
-      <c r="AC15" s="3">
-        <v>18.183040637561799</v>
-      </c>
-      <c r="AD15" s="3">
+      <c r="AA15">
+        <v>0.346394732182703</v>
+      </c>
+      <c r="AB15" s="8">
+        <v>44858</v>
+      </c>
+      <c r="AC15">
+        <v>0.346394732182703</v>
+      </c>
+      <c r="AD15">
         <f t="shared" si="20"/>
-        <v>1.6590004852178608</v>
-      </c>
-      <c r="AE15" s="3">
+        <v>0.29040534914420774</v>
+      </c>
+      <c r="AE15">
         <f t="shared" si="21"/>
-        <v>30.165673240451106</v>
-      </c>
-      <c r="AF15" s="3">
-        <v>43.9911339197808</v>
-      </c>
-      <c r="AG15" s="3">
-        <v>43.756112180507998</v>
-      </c>
-      <c r="AH15" s="3">
-        <v>2.1366413312415702</v>
-      </c>
-      <c r="AI15" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="3" t="str">
+        <v>0.1005948831412322</v>
+      </c>
+      <c r="AF15">
+        <v>1.85368192555823</v>
+      </c>
+      <c r="AG15">
+        <v>1.71494163231468</v>
+      </c>
+      <c r="AH15">
+        <v>1.24626443820073</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15" t="str">
         <f t="shared" si="22"/>
         <v>NA</v>
       </c>
-      <c r="AK15" s="3">
+      <c r="AK15">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AL15" s="3">
-        <v>18.183040637561799</v>
+      <c r="AL15">
+        <v>0.346394732182703</v>
       </c>
     </row>
-    <row r="16" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>44909</v>
-      </c>
-      <c r="B16" s="3">
-        <v>5.7</v>
-      </c>
-      <c r="C16" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1.355375</v>
-      </c>
-      <c r="F16" s="2">
-        <v>44909</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1.1681465035976</v>
-      </c>
-      <c r="H16" s="3">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>44859</v>
+      </c>
+      <c r="B16">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C16">
+        <v>3.2</v>
+      </c>
+      <c r="D16">
+        <v>1.2825</v>
+      </c>
+      <c r="F16" s="8">
+        <v>44859</v>
+      </c>
+      <c r="G16">
+        <v>9.8783657954231394</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="12"/>
-        <v>0.49578349745769312</v>
-      </c>
-      <c r="I16" s="3">
+        <v>1.2683955062330992</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="13"/>
-        <v>0.57914775909659377</v>
-      </c>
-      <c r="J16" s="3">
-        <v>57.994429062441398</v>
-      </c>
-      <c r="K16" s="3">
-        <v>3.33505853945065</v>
-      </c>
-      <c r="L16" s="3">
+        <v>12.529674783841465</v>
+      </c>
+      <c r="J16">
+        <v>60.000006268762498</v>
+      </c>
+      <c r="K16">
+        <v>21.531600006132599</v>
+      </c>
+      <c r="L16">
         <v>5</v>
       </c>
-      <c r="M16" s="3">
-        <v>0</v>
-      </c>
-      <c r="N16" s="3">
+      <c r="M16">
+        <v>1.0447094609844501</v>
+      </c>
+      <c r="N16">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="3" t="str">
+        <v>0.47201008851963605</v>
+      </c>
+      <c r="O16">
         <f t="shared" si="15"/>
-        <v>NA</v>
-      </c>
-      <c r="P16" s="3">
-        <v>1.1681465035976</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>44909</v>
-      </c>
-      <c r="R16" s="3">
-        <v>1.1681465035976</v>
-      </c>
-      <c r="S16" s="3">
+        <v>0.49311340515657154</v>
+      </c>
+      <c r="P16">
+        <v>8.8359427507619195</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>44859</v>
+      </c>
+      <c r="R16">
+        <v>8.8359427507619195</v>
+      </c>
+      <c r="S16">
         <f t="shared" si="16"/>
-        <v>0.49578349745769312</v>
-      </c>
-      <c r="T16" s="3">
+        <v>1.2076595554533669</v>
+      </c>
+      <c r="T16">
         <f t="shared" si="17"/>
-        <v>0.57914775909659377</v>
-      </c>
-      <c r="U16" s="3">
-        <v>37.3597013593239</v>
-      </c>
-      <c r="V16" s="3">
-        <v>3.33505853945065</v>
-      </c>
-      <c r="W16" s="3">
+        <v>10.67081069439654</v>
+      </c>
+      <c r="U16">
+        <v>33.381313742145402</v>
+      </c>
+      <c r="V16">
+        <v>21.531600006132599</v>
+      </c>
+      <c r="W16">
         <v>10</v>
       </c>
-      <c r="X16" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="3" t="str">
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="str">
         <f t="shared" si="18"/>
         <v>NA</v>
       </c>
-      <c r="Z16" s="3">
+      <c r="Z16">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AA16" s="3">
-        <v>1.1681465035976</v>
-      </c>
-      <c r="AB16" s="2">
-        <v>44909</v>
-      </c>
-      <c r="AC16" s="3">
-        <v>1.1681465035976</v>
-      </c>
-      <c r="AD16" s="3">
+      <c r="AA16">
+        <v>8.8359427507619195</v>
+      </c>
+      <c r="AB16" s="8">
+        <v>44859</v>
+      </c>
+      <c r="AC16">
+        <v>8.8359427507619195</v>
+      </c>
+      <c r="AD16">
         <f t="shared" si="20"/>
-        <v>0.49578349745769312</v>
-      </c>
-      <c r="AE16" s="3">
+        <v>1.2076595554533669</v>
+      </c>
+      <c r="AE16">
         <f t="shared" si="21"/>
-        <v>0.57914775909659377</v>
-      </c>
-      <c r="AF16" s="3">
-        <v>27.326875631122299</v>
-      </c>
-      <c r="AG16" s="3">
-        <v>3.33505853945065</v>
-      </c>
-      <c r="AH16" s="3">
-        <v>20</v>
-      </c>
-      <c r="AI16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="3" t="str">
+        <v>10.67081069439654</v>
+      </c>
+      <c r="AF16">
+        <v>21.717601628735899</v>
+      </c>
+      <c r="AG16">
+        <v>21.531600006132599</v>
+      </c>
+      <c r="AH16">
+        <v>1.6683137330024</v>
+      </c>
+      <c r="AI16">
+        <v>0</v>
+      </c>
+      <c r="AJ16" t="str">
         <f t="shared" si="22"/>
         <v>NA</v>
       </c>
-      <c r="AK16" s="3">
+      <c r="AK16">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AL16" s="3">
-        <v>1.1681465035976</v>
+      <c r="AL16">
+        <v>8.8359427507619195</v>
       </c>
     </row>
-    <row r="17" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>44910</v>
-      </c>
-      <c r="B17" s="3">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>44860</v>
+      </c>
+      <c r="B17">
+        <v>4.7</v>
+      </c>
+      <c r="C17">
         <v>2</v>
       </c>
-      <c r="C17" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1.3665</v>
-      </c>
-      <c r="F17" s="2">
-        <v>44910</v>
-      </c>
-      <c r="G17" s="3">
-        <v>11.174497457821801</v>
-      </c>
-      <c r="H17" s="3">
+      <c r="D17">
+        <v>1.1472500000000001</v>
+      </c>
+      <c r="F17" s="8">
+        <v>44860</v>
+      </c>
+      <c r="G17">
+        <v>6.4880518783200101</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="12"/>
-        <v>1.3391017247082451</v>
-      </c>
-      <c r="I17" s="3">
+        <v>1.0542012989893934</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="13"/>
-        <v>14.963788818517074</v>
-      </c>
-      <c r="J17" s="3">
-        <v>60.000035244217301</v>
-      </c>
-      <c r="K17" s="3">
-        <v>12.8824400179849</v>
-      </c>
-      <c r="L17" s="3">
+        <v>6.8397127180355284</v>
+      </c>
+      <c r="J17">
+        <v>60.000019402708702</v>
+      </c>
+      <c r="K17">
+        <v>8.2304722383888702</v>
+      </c>
+      <c r="L17">
         <v>5</v>
       </c>
-      <c r="M17" s="3">
-        <v>5.87408383459357</v>
-      </c>
-      <c r="N17" s="3">
+      <c r="M17">
+        <v>3.2338341055340898</v>
+      </c>
+      <c r="N17">
         <f t="shared" si="14"/>
-        <v>1.0090830489105456</v>
-      </c>
-      <c r="O17" s="3">
+        <v>0.77601310089374531</v>
+      </c>
+      <c r="O17">
         <f t="shared" si="15"/>
-        <v>5.9274384253678285</v>
-      </c>
-      <c r="P17" s="3">
-        <v>5.3150693081640998</v>
-      </c>
-      <c r="Q17" s="2">
-        <v>44910</v>
-      </c>
-      <c r="R17" s="3">
-        <v>5.3150693081640998</v>
-      </c>
-      <c r="S17" s="3">
+        <v>2.5094976320114601</v>
+      </c>
+      <c r="P17">
+        <v>3.2533740430396998</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>44860</v>
+      </c>
+      <c r="R17">
+        <v>3.2533740430396998</v>
+      </c>
+      <c r="S17">
         <f t="shared" si="16"/>
-        <v>0.96564429501665683</v>
-      </c>
-      <c r="T17" s="3">
+        <v>0.77807275399737807</v>
+      </c>
+      <c r="T17">
         <f t="shared" si="17"/>
-        <v>5.1324663550467919</v>
-      </c>
-      <c r="U17" s="3">
-        <v>40.240297030361504</v>
-      </c>
-      <c r="V17" s="3">
-        <v>12.8824400179849</v>
-      </c>
-      <c r="W17" s="3">
+        <v>2.5313617014514835</v>
+      </c>
+      <c r="U17">
+        <v>31.613564243522902</v>
+      </c>
+      <c r="V17">
+        <v>8.2304722383888702</v>
+      </c>
+      <c r="W17">
         <v>10</v>
       </c>
-      <c r="X17" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="3" t="str">
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="str">
         <f t="shared" si="18"/>
         <v>NA</v>
       </c>
-      <c r="Z17" s="3">
+      <c r="Z17">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AA17" s="3">
-        <v>5.3150693081640998</v>
-      </c>
-      <c r="AB17" s="2">
-        <v>44910</v>
-      </c>
-      <c r="AC17" s="3">
-        <v>5.3150693081640998</v>
-      </c>
-      <c r="AD17" s="3">
+      <c r="AA17">
+        <v>3.2533740430396998</v>
+      </c>
+      <c r="AB17" s="8">
+        <v>44860</v>
+      </c>
+      <c r="AC17">
+        <v>3.2533740430396998</v>
+      </c>
+      <c r="AD17">
         <f t="shared" si="20"/>
-        <v>0.96564429501665683</v>
-      </c>
-      <c r="AE17" s="3">
+        <v>0.77807275399737807</v>
+      </c>
+      <c r="AE17">
         <f t="shared" si="21"/>
-        <v>5.1324663550467919</v>
-      </c>
-      <c r="AF17" s="3">
-        <v>20.208389431258201</v>
-      </c>
-      <c r="AG17" s="3">
-        <v>12.8824400179849</v>
-      </c>
-      <c r="AH17" s="3">
-        <v>20</v>
-      </c>
-      <c r="AI17" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="3" t="str">
+        <v>2.5313617014514835</v>
+      </c>
+      <c r="AF17">
+        <v>10.402817559750201</v>
+      </c>
+      <c r="AG17">
+        <v>8.2304722383888702</v>
+      </c>
+      <c r="AH17">
+        <v>19.545841465862299</v>
+      </c>
+      <c r="AI17">
+        <v>0</v>
+      </c>
+      <c r="AJ17" t="str">
         <f t="shared" si="22"/>
         <v>NA</v>
       </c>
-      <c r="AK17" s="3">
+      <c r="AK17">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AL17" s="3">
-        <v>5.3150693081640998</v>
+      <c r="AL17">
+        <v>3.2533740430396998</v>
       </c>
     </row>
-    <row r="18" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>44911</v>
-      </c>
-      <c r="B18" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="C18" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1.24325</v>
-      </c>
-      <c r="F18" s="2">
-        <v>44911</v>
-      </c>
-      <c r="G18" s="3">
-        <v>1.26273678391016</v>
-      </c>
-      <c r="H18" s="3">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
+        <v>44861</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D18">
+        <v>0.76137500000000002</v>
+      </c>
+      <c r="F18" s="8">
+        <v>44861</v>
+      </c>
+      <c r="G18">
+        <v>10.8714053659413</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="12"/>
-        <v>0.51306323470546977</v>
-      </c>
-      <c r="I18" s="3">
+        <v>1.3229972833896266</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="13"/>
-        <v>0.64786381893452849</v>
-      </c>
-      <c r="J18" s="3">
-        <v>58.114500348013202</v>
-      </c>
-      <c r="K18" s="3">
-        <v>3.1213662007122598</v>
-      </c>
-      <c r="L18" s="3">
+        <v>14.382839765767748</v>
+      </c>
+      <c r="J18">
+        <v>60.000039869841601</v>
+      </c>
+      <c r="K18">
+        <v>11.634086733313801</v>
+      </c>
+      <c r="L18">
         <v>5</v>
       </c>
-      <c r="M18" s="3">
-        <v>0</v>
-      </c>
-      <c r="N18" s="3">
+      <c r="M18">
+        <v>6.6449412734073103</v>
+      </c>
+      <c r="N18">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="3" t="str">
+        <v>1.0653427474129673</v>
+      </c>
+      <c r="O18">
         <f t="shared" si="15"/>
-        <v>NA</v>
-      </c>
-      <c r="P18" s="3">
-        <v>1.26273678391016</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>44911</v>
-      </c>
-      <c r="R18" s="3">
-        <v>1.26273678391016</v>
-      </c>
-      <c r="S18" s="3">
+        <v>7.0791399926095657</v>
+      </c>
+      <c r="P18">
+        <v>4.2237453509359204</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>44861</v>
+      </c>
+      <c r="R18">
+        <v>4.2237453509359204</v>
+      </c>
+      <c r="S18">
         <f t="shared" si="16"/>
-        <v>0.51306323470546977</v>
-      </c>
-      <c r="T18" s="3">
+        <v>0.87277088225189403</v>
+      </c>
+      <c r="T18">
         <f t="shared" si="17"/>
-        <v>0.64786381893452849</v>
-      </c>
-      <c r="U18" s="3">
-        <v>33.357702003960803</v>
-      </c>
-      <c r="V18" s="3">
-        <v>3.1213662007122598</v>
-      </c>
-      <c r="W18" s="3">
+        <v>3.6863619563436791</v>
+      </c>
+      <c r="U18">
+        <v>33.2536782060116</v>
+      </c>
+      <c r="V18">
+        <v>11.634086733313801</v>
+      </c>
+      <c r="W18">
         <v>10</v>
       </c>
-      <c r="X18" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="3" t="str">
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="str">
         <f t="shared" si="18"/>
         <v>NA</v>
       </c>
-      <c r="Z18" s="3">
+      <c r="Z18">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AA18" s="3">
-        <v>1.26273678391016</v>
-      </c>
-      <c r="AB18" s="2">
-        <v>44911</v>
-      </c>
-      <c r="AC18" s="3">
-        <v>1.26273678391016</v>
-      </c>
-      <c r="AD18" s="3">
+      <c r="AA18">
+        <v>4.2237453509359204</v>
+      </c>
+      <c r="AB18" s="8">
+        <v>44861</v>
+      </c>
+      <c r="AC18">
+        <v>4.2237453509359204</v>
+      </c>
+      <c r="AD18">
         <f t="shared" si="20"/>
-        <v>0.51306323470546977</v>
-      </c>
-      <c r="AE18" s="3">
+        <v>0.87277088225189403</v>
+      </c>
+      <c r="AE18">
         <f t="shared" si="21"/>
-        <v>0.64786381893452849</v>
-      </c>
-      <c r="AF18" s="3">
-        <v>5.1415945794817599</v>
-      </c>
-      <c r="AG18" s="3">
-        <v>3.1213662007122598</v>
-      </c>
-      <c r="AH18" s="3">
-        <v>18.187550488132398</v>
-      </c>
-      <c r="AI18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="3" t="str">
+        <v>3.6863619563436791</v>
+      </c>
+      <c r="AF18">
+        <v>12.676666135025799</v>
+      </c>
+      <c r="AG18">
+        <v>11.634086733313801</v>
+      </c>
+      <c r="AH18">
+        <v>9.3625358037751703</v>
+      </c>
+      <c r="AI18">
+        <v>0</v>
+      </c>
+      <c r="AJ18" t="str">
         <f t="shared" si="22"/>
         <v>NA</v>
       </c>
-      <c r="AK18" s="3">
+      <c r="AK18">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AL18" s="3">
-        <v>1.26273678391016</v>
+      <c r="AL18">
+        <v>4.2237453509359204</v>
       </c>
     </row>
-    <row r="19" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>44912</v>
-      </c>
-      <c r="B19" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="C19" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1.3532500000000001</v>
-      </c>
-      <c r="F19" s="2">
-        <v>44912</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.90797919327864196</v>
-      </c>
-      <c r="H19" s="3">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>44862</v>
+      </c>
+      <c r="B19">
+        <v>1.9</v>
+      </c>
+      <c r="C19">
+        <v>2.5</v>
+      </c>
+      <c r="D19">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="F19" s="8">
+        <v>44862</v>
+      </c>
+      <c r="G19">
+        <v>46.246753671594803</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="12"/>
-        <v>0.4437584576703642</v>
-      </c>
-      <c r="I19" s="3">
+        <v>2.5016641216006437</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="13"/>
-        <v>0.40292344640611166</v>
-      </c>
-      <c r="J19" s="3">
-        <v>55.352020250693599</v>
-      </c>
-      <c r="K19" s="3">
-        <v>2.2444389052117502</v>
-      </c>
-      <c r="L19" s="3">
+        <v>115.69384440073155</v>
+      </c>
+      <c r="J19">
+        <v>60.000187655595802</v>
+      </c>
+      <c r="K19">
+        <v>36.276860032256501</v>
+      </c>
+      <c r="L19">
         <v>5</v>
       </c>
-      <c r="M19" s="3">
-        <v>0</v>
-      </c>
-      <c r="N19" s="3">
+      <c r="M19">
+        <v>31.275962244156599</v>
+      </c>
+      <c r="N19">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="3" t="str">
+        <v>2.1061337530280175</v>
+      </c>
+      <c r="O19">
         <f t="shared" si="15"/>
-        <v>NA</v>
-      </c>
-      <c r="P19" s="3">
-        <v>0.90797919327864196</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>44912</v>
-      </c>
-      <c r="R19" s="3">
-        <v>0.90797919327864196</v>
-      </c>
-      <c r="S19" s="3">
+        <v>65.871359740848121</v>
+      </c>
+      <c r="P19">
+        <v>14.970978910675999</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>44862</v>
+      </c>
+      <c r="R19">
+        <v>14.970978910675999</v>
+      </c>
+      <c r="S19">
         <f t="shared" si="16"/>
-        <v>0.4437584576703642</v>
-      </c>
-      <c r="T19" s="3">
+        <v>1.5230120389267607</v>
+      </c>
+      <c r="T19">
         <f t="shared" si="17"/>
-        <v>0.40292344640611166</v>
-      </c>
-      <c r="U19" s="3">
-        <v>25.5989410415424</v>
-      </c>
-      <c r="V19" s="3">
-        <v>2.2444389052117502</v>
-      </c>
-      <c r="W19" s="3">
+        <v>22.800981115478187</v>
+      </c>
+      <c r="U19">
+        <v>59.529794115841597</v>
+      </c>
+      <c r="V19">
+        <v>36.276860032256501</v>
+      </c>
+      <c r="W19">
         <v>10</v>
       </c>
-      <c r="X19" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="3" t="str">
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="str">
         <f t="shared" si="18"/>
         <v>NA</v>
       </c>
-      <c r="Z19" s="3">
+      <c r="Z19">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AA19" s="3">
-        <v>0.90797919327864196</v>
-      </c>
-      <c r="AB19" s="2">
-        <v>44912</v>
-      </c>
-      <c r="AC19" s="3">
-        <v>0.90797919327864196</v>
-      </c>
-      <c r="AD19" s="3">
+      <c r="AA19">
+        <v>14.970978910675999</v>
+      </c>
+      <c r="AB19" s="8">
+        <v>44862</v>
+      </c>
+      <c r="AC19">
+        <v>14.970978910675999</v>
+      </c>
+      <c r="AD19">
         <f t="shared" si="20"/>
-        <v>0.4437584576703642</v>
-      </c>
-      <c r="AE19" s="3">
+        <v>1.5230120389267607</v>
+      </c>
+      <c r="AE19">
         <f t="shared" si="21"/>
-        <v>0.40292344640611166</v>
-      </c>
-      <c r="AF19" s="3">
-        <v>2.75825358146224</v>
-      </c>
-      <c r="AG19" s="3">
-        <v>2.2444389052117502</v>
-      </c>
-      <c r="AH19" s="3">
-        <v>4.6274351215335896</v>
-      </c>
-      <c r="AI19" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ19" s="3" t="str">
+        <v>22.800981115478187</v>
+      </c>
+      <c r="AF19">
+        <v>37.544057345042297</v>
+      </c>
+      <c r="AG19">
+        <v>36.276860032256501</v>
+      </c>
+      <c r="AH19">
+        <v>11.408999521523199</v>
+      </c>
+      <c r="AI19">
+        <v>0</v>
+      </c>
+      <c r="AJ19" t="str">
         <f t="shared" si="22"/>
         <v>NA</v>
       </c>
-      <c r="AK19" s="3">
+      <c r="AK19">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AL19" s="3">
-        <v>0.90797919327864196</v>
+      <c r="AL19">
+        <v>14.970978910675999</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>45202</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1.9</v>
+      </c>
+      <c r="F23" s="8">
+        <v>45202</v>
+      </c>
+      <c r="G23">
+        <v>1.52562178492945E-4</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23:H29" si="24">EXP(0.44*LN(G23)-0.77)</f>
+        <v>9.6896898621207719E-3</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ref="I23:I29" si="25">H23*G23</f>
+        <v>1.4782801942861487E-6</v>
+      </c>
+      <c r="J23">
+        <v>5.1424174240730699E-4</v>
+      </c>
+      <c r="K23">
+        <v>3.7711931221351701E-4</v>
+      </c>
+      <c r="L23">
+        <v>1.2342850703648499E-3</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ref="N23:N29" si="26">IF(M23=0,0,EXP(0.44*LN(M23)-0.77))</f>
+        <v>0</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" ref="O23:O29" si="27">IF(M23=0,"NA",N23*M23)</f>
+        <v>NA</v>
+      </c>
+      <c r="P23">
+        <v>1.52562178492945E-4</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>45202</v>
+      </c>
+      <c r="R23">
+        <v>1.52562178492945E-4</v>
+      </c>
+      <c r="S23">
+        <f t="shared" ref="S23:S29" si="28">EXP(0.44*LN(R23)-0.77)</f>
+        <v>9.6896898621207719E-3</v>
+      </c>
+      <c r="T23">
+        <f t="shared" ref="T23:T29" si="29">S23*R23</f>
+        <v>1.4782801942861487E-6</v>
+      </c>
+      <c r="U23">
+        <v>5.1424174240730699E-4</v>
+      </c>
+      <c r="V23">
+        <v>3.7711931221351701E-4</v>
+      </c>
+      <c r="W23">
+        <v>1.2342850703648499E-3</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="str">
+        <f t="shared" ref="Y23:Y29" si="30">IF(X23=0,"NA",EXP(0.44*LN(X23)-0.77))</f>
+        <v>NA</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" ref="Z23:Z29" si="31">IF(X23=0,0,Y23*X23)</f>
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>1.52562178492945E-4</v>
+      </c>
+      <c r="AB23" s="8">
+        <v>45202</v>
+      </c>
+      <c r="AC23">
+        <v>1.52562178492945E-4</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" ref="AD23:AD29" si="32">EXP(0.44*LN(AC23)-0.77)</f>
+        <v>9.6896898621207719E-3</v>
+      </c>
+      <c r="AE23">
+        <f t="shared" ref="AE23:AE29" si="33">AD23*AC23</f>
+        <v>1.4782801942861487E-6</v>
+      </c>
+      <c r="AF23">
+        <v>5.1424174240730699E-4</v>
+      </c>
+      <c r="AG23">
+        <v>3.7711931221351701E-4</v>
+      </c>
+      <c r="AH23">
+        <v>1.2342850703648499E-3</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23" t="str">
+        <f t="shared" ref="AJ23:AJ29" si="34">IF(AI23=0,"NA",EXP(0.44*LN(AI23)-0.77))</f>
+        <v>NA</v>
+      </c>
+      <c r="AK23">
+        <f t="shared" ref="AK23:AK29" si="35">IF(AI23=0,0,AJ23*AI23)</f>
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>1.52562178492945E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>45203</v>
+      </c>
+      <c r="B24">
+        <v>105</v>
+      </c>
+      <c r="C24">
+        <v>2.1</v>
+      </c>
+      <c r="F24" s="8">
+        <v>45203</v>
+      </c>
+      <c r="G24">
+        <v>1.0970083830448699E-4</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="24"/>
+        <v>8.3808028672864854E-3</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="25"/>
+        <v>9.1938110020597574E-7</v>
+      </c>
+      <c r="J24">
+        <v>18.380544277816899</v>
+      </c>
+      <c r="K24">
+        <v>18.3406267442789</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="P24">
+        <v>1.0970083830448699E-4</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>45203</v>
+      </c>
+      <c r="R24">
+        <v>1.0970083830448699E-4</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="28"/>
+        <v>8.3808028672864854E-3</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="29"/>
+        <v>9.1938110020597574E-7</v>
+      </c>
+      <c r="U24">
+        <v>18.380544277816899</v>
+      </c>
+      <c r="V24">
+        <v>18.3406267442789</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>1.0970083830448699E-4</v>
+      </c>
+      <c r="AB24" s="8">
+        <v>45203</v>
+      </c>
+      <c r="AC24">
+        <v>1.0970083830448699E-4</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="32"/>
+        <v>8.3808028672864854E-3</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" si="33"/>
+        <v>9.1938110020597574E-7</v>
+      </c>
+      <c r="AF24">
+        <v>18.380544277816899</v>
+      </c>
+      <c r="AG24">
+        <v>18.3406267442789</v>
+      </c>
+      <c r="AH24">
+        <v>0</v>
+      </c>
+      <c r="AI24">
+        <v>0</v>
+      </c>
+      <c r="AJ24" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="AK24">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="AL24">
+        <v>1.0970083830448699E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>45204</v>
+      </c>
+      <c r="B25">
+        <v>31.5</v>
+      </c>
+      <c r="C25">
+        <v>3.1</v>
+      </c>
+      <c r="F25" s="8">
+        <v>45204</v>
+      </c>
+      <c r="G25">
+        <v>595.61809050623197</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="24"/>
+        <v>7.7015673225534638</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="25"/>
+        <v>4587.1928225644879</v>
+      </c>
+      <c r="J25">
+        <v>60.002473174521597</v>
+      </c>
+      <c r="K25">
+        <v>458.782130782835</v>
+      </c>
+      <c r="L25">
+        <v>5</v>
+      </c>
+      <c r="M25">
+        <v>412.195703349425</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="26"/>
+        <v>6.5499618661433274</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="27"/>
+        <v>2699.8661383268613</v>
+      </c>
+      <c r="P25">
+        <v>183.40363462267001</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>45204</v>
+      </c>
+      <c r="R25">
+        <v>530.63522752722497</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="28"/>
+        <v>7.3198726172263289</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="29"/>
+        <v>3884.1822717121968</v>
+      </c>
+      <c r="U25">
+        <v>120.00208338876899</v>
+      </c>
+      <c r="V25">
+        <v>458.782130782835</v>
+      </c>
+      <c r="W25">
+        <v>10</v>
+      </c>
+      <c r="X25">
+        <v>347.23159290455499</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="30"/>
+        <v>6.0738730612374701</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="31"/>
+        <v>2109.0406181535523</v>
+      </c>
+      <c r="AA25">
+        <v>183.40363462267001</v>
+      </c>
+      <c r="AB25" s="8">
+        <v>45204</v>
+      </c>
+      <c r="AC25">
+        <v>404.20098375883703</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="32"/>
+        <v>6.4937578523138546</v>
+      </c>
+      <c r="AE25">
+        <f t="shared" si="33"/>
+        <v>2624.7833121969329</v>
+      </c>
+      <c r="AF25">
+        <v>240.001324565169</v>
+      </c>
+      <c r="AG25">
+        <v>458.782130782835</v>
+      </c>
+      <c r="AH25">
+        <v>16.542489850035199</v>
+      </c>
+      <c r="AI25">
+        <v>220.76086143109299</v>
+      </c>
+      <c r="AJ25">
+        <f t="shared" si="34"/>
+        <v>4.9764421992586456</v>
+      </c>
+      <c r="AK25">
+        <f t="shared" si="35"/>
+        <v>1098.6036667703816</v>
+      </c>
+      <c r="AL25">
+        <v>183.40363462267001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>45205</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="F26" s="2">
+        <v>45205</v>
+      </c>
+      <c r="G26" s="3">
+        <v>636.93534142865201</v>
+      </c>
+      <c r="H26" s="3">
+        <f t="shared" si="24"/>
+        <v>7.9322282339386589</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="25"/>
+        <v>5052.3164984737132</v>
+      </c>
+      <c r="J26" s="3">
+        <v>60.002704811584302</v>
+      </c>
+      <c r="K26" s="3">
+        <v>455.80462120673701</v>
+      </c>
+      <c r="L26" s="3">
+        <v>5</v>
+      </c>
+      <c r="M26" s="3">
+        <v>450.80188945697302</v>
+      </c>
+      <c r="N26" s="3">
+        <f t="shared" si="26"/>
+        <v>6.8131346026908677</v>
+      </c>
+      <c r="O26" s="3">
+        <f t="shared" si="27"/>
+        <v>3071.3739520177264</v>
+      </c>
+      <c r="P26" s="3">
+        <v>186.134076884275</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>45205</v>
+      </c>
+      <c r="R26" s="3">
+        <v>631.93310657493998</v>
+      </c>
+      <c r="S26" s="3">
+        <f t="shared" si="28"/>
+        <v>7.9047572326916669</v>
+      </c>
+      <c r="T26" s="3">
+        <f t="shared" si="29"/>
+        <v>4995.2777947755703</v>
+      </c>
+      <c r="U26" s="3">
+        <v>120.00267479339099</v>
+      </c>
+      <c r="V26" s="3">
+        <v>455.80462120673701</v>
+      </c>
+      <c r="W26" s="3">
+        <v>10</v>
+      </c>
+      <c r="X26" s="3">
+        <v>445.79902969066501</v>
+      </c>
+      <c r="Y26" s="3">
+        <f t="shared" si="30"/>
+        <v>6.7797621996036641</v>
+      </c>
+      <c r="Z26" s="3">
+        <f t="shared" si="31"/>
+        <v>3022.411410116762</v>
+      </c>
+      <c r="AA26" s="3">
+        <v>186.134076884275</v>
+      </c>
+      <c r="AB26" s="2">
+        <v>45205</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>621.92490799584095</v>
+      </c>
+      <c r="AD26" s="3">
+        <f t="shared" si="32"/>
+        <v>7.8494268614828027</v>
+      </c>
+      <c r="AE26" s="3">
+        <f t="shared" si="33"/>
+        <v>4881.7540786477748</v>
+      </c>
+      <c r="AF26" s="3">
+        <v>240.00261476033501</v>
+      </c>
+      <c r="AG26" s="3">
+        <v>455.80462120673701</v>
+      </c>
+      <c r="AH26" s="3">
+        <v>20</v>
+      </c>
+      <c r="AI26" s="3">
+        <v>435.79333090262202</v>
+      </c>
+      <c r="AJ26" s="3">
+        <f t="shared" si="34"/>
+        <v>6.7123826171738097</v>
+      </c>
+      <c r="AK26" s="3">
+        <f t="shared" si="35"/>
+        <v>2925.211579031034</v>
+      </c>
+      <c r="AL26" s="3">
+        <v>186.134076884275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>45206</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3</v>
+      </c>
+      <c r="F27" s="2">
+        <v>45206</v>
+      </c>
+      <c r="G27" s="3">
+        <v>310.34437711701202</v>
+      </c>
+      <c r="H27" s="3">
+        <f t="shared" si="24"/>
+        <v>5.7810211285530979</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="25"/>
+        <v>1794.107401241097</v>
+      </c>
+      <c r="J27" s="3">
+        <v>60.001317101203398</v>
+      </c>
+      <c r="K27" s="3">
+        <v>224.51915391047001</v>
+      </c>
+      <c r="L27" s="3">
+        <v>5</v>
+      </c>
+      <c r="M27" s="3">
+        <v>219.516916541276</v>
+      </c>
+      <c r="N27" s="3">
+        <f t="shared" si="26"/>
+        <v>4.9640845069060981</v>
+      </c>
+      <c r="O27" s="3">
+        <f t="shared" si="27"/>
+        <v>1089.7005244063471</v>
+      </c>
+      <c r="P27" s="3">
+        <v>90.828366844763295</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>45206</v>
+      </c>
+      <c r="R27" s="3">
+        <v>305.34165839085199</v>
+      </c>
+      <c r="S27" s="3">
+        <f t="shared" si="28"/>
+        <v>5.7398311302801348</v>
+      </c>
+      <c r="T27" s="3">
+        <f t="shared" si="29"/>
+        <v>1752.6095562031749</v>
+      </c>
+      <c r="U27" s="3">
+        <v>120.001287080011</v>
+      </c>
+      <c r="V27" s="3">
+        <v>224.51915391047001</v>
+      </c>
+      <c r="W27" s="3">
+        <v>10</v>
+      </c>
+      <c r="X27" s="3">
+        <v>214.51329154608899</v>
+      </c>
+      <c r="Y27" s="3">
+        <f t="shared" si="30"/>
+        <v>4.9139767796760818</v>
+      </c>
+      <c r="Z27" s="3">
+        <f t="shared" si="31"/>
+        <v>1054.1133335893669</v>
+      </c>
+      <c r="AA27" s="3">
+        <v>90.828366844763295</v>
+      </c>
+      <c r="AB27" s="2">
+        <v>45206</v>
+      </c>
+      <c r="AC27" s="3">
+        <v>295.330783391414</v>
+      </c>
+      <c r="AD27" s="3">
+        <f t="shared" si="32"/>
+        <v>5.6562563562667334</v>
+      </c>
+      <c r="AE27" s="3">
+        <f t="shared" si="33"/>
+        <v>1670.4666207589194</v>
+      </c>
+      <c r="AF27" s="3">
+        <v>240.00122703696999</v>
+      </c>
+      <c r="AG27" s="3">
+        <v>224.51915391047001</v>
+      </c>
+      <c r="AH27" s="3">
+        <v>20</v>
+      </c>
+      <c r="AI27" s="3">
+        <v>204.506041559701</v>
+      </c>
+      <c r="AJ27" s="3">
+        <f t="shared" si="34"/>
+        <v>4.8117599346486353</v>
+      </c>
+      <c r="AK27" s="3">
+        <f t="shared" si="35"/>
+        <v>984.03397717055805</v>
+      </c>
+      <c r="AL27" s="3">
+        <v>90.828366844763295</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>45207</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="F28" s="2">
+        <v>45207</v>
+      </c>
+      <c r="G28" s="3">
+        <v>221.74777567664199</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="24"/>
+        <v>4.9862187638585178</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="25"/>
+        <v>1105.6829199227618</v>
+      </c>
+      <c r="J28" s="3">
+        <v>60.000938628445702</v>
+      </c>
+      <c r="K28" s="3">
+        <v>161.44197495535599</v>
+      </c>
+      <c r="L28" s="3">
+        <v>5</v>
+      </c>
+      <c r="M28" s="3">
+        <v>156.43810336162801</v>
+      </c>
+      <c r="N28" s="3">
+        <f t="shared" si="26"/>
+        <v>4.2766525430482618</v>
+      </c>
+      <c r="O28" s="3">
+        <f t="shared" si="27"/>
+        <v>669.03141257115328</v>
+      </c>
+      <c r="P28" s="3">
+        <v>65.310734830380895</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>45207</v>
+      </c>
+      <c r="R28" s="3">
+        <v>216.74458819706601</v>
+      </c>
+      <c r="S28" s="3">
+        <f t="shared" si="28"/>
+        <v>4.9364016006729265</v>
+      </c>
+      <c r="T28" s="3">
+        <f t="shared" si="29"/>
+        <v>1069.9383321131909</v>
+      </c>
+      <c r="U28" s="3">
+        <v>120.00090860312</v>
+      </c>
+      <c r="V28" s="3">
+        <v>161.44197495535599</v>
+      </c>
+      <c r="W28" s="3">
+        <v>10</v>
+      </c>
+      <c r="X28" s="3">
+        <v>151.43385336668501</v>
+      </c>
+      <c r="Y28" s="3">
+        <f t="shared" si="30"/>
+        <v>4.2159102539257649</v>
+      </c>
+      <c r="Z28" s="3">
+        <f t="shared" si="31"/>
+        <v>638.4315352000981</v>
+      </c>
+      <c r="AA28" s="3">
+        <v>65.310734830380895</v>
+      </c>
+      <c r="AB28" s="2">
+        <v>45207</v>
+      </c>
+      <c r="AC28" s="3">
+        <v>206.73183820017499</v>
+      </c>
+      <c r="AD28" s="3">
+        <f t="shared" si="32"/>
+        <v>4.8347329453876986</v>
+      </c>
+      <c r="AE28" s="3">
+        <f t="shared" si="33"/>
+        <v>999.49322900694517</v>
+      </c>
+      <c r="AF28" s="3">
+        <v>240.00084855212</v>
+      </c>
+      <c r="AG28" s="3">
+        <v>161.44197495535599</v>
+      </c>
+      <c r="AH28" s="3">
+        <v>20</v>
+      </c>
+      <c r="AI28" s="3">
+        <v>141.42535337790201</v>
+      </c>
+      <c r="AJ28" s="3">
+        <f t="shared" si="34"/>
+        <v>4.0909601481999447</v>
+      </c>
+      <c r="AK28" s="3">
+        <f t="shared" si="35"/>
+        <v>578.56548461409159</v>
+      </c>
+      <c r="AL28" s="3">
+        <v>65.310734830380895</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>45208</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="F29" s="2">
+        <v>45208</v>
+      </c>
+      <c r="G29" s="3">
+        <v>158.04220632858701</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" si="24"/>
+        <v>4.2958925078666725</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="25"/>
+        <v>678.93233009369578</v>
+      </c>
+      <c r="J29" s="3">
+        <v>60.000666488265999</v>
+      </c>
+      <c r="K29" s="3">
+        <v>116.085914379844</v>
+      </c>
+      <c r="L29" s="3">
+        <v>5</v>
+      </c>
+      <c r="M29" s="3">
+        <v>111.08131146587201</v>
+      </c>
+      <c r="N29" s="3">
+        <f t="shared" si="26"/>
+        <v>3.678538351915559</v>
+      </c>
+      <c r="O29" s="3">
+        <f t="shared" si="27"/>
+        <v>408.61686440828771</v>
+      </c>
+      <c r="P29" s="3">
+        <v>46.962113624420603</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>45208</v>
+      </c>
+      <c r="R29" s="3">
+        <v>153.03855009797701</v>
+      </c>
+      <c r="S29" s="3">
+        <f t="shared" si="28"/>
+        <v>4.2355091045804736</v>
+      </c>
+      <c r="T29" s="3">
+        <f t="shared" si="29"/>
+        <v>648.19617229177652</v>
+      </c>
+      <c r="U29" s="3">
+        <v>120.000636457696</v>
+      </c>
+      <c r="V29" s="3">
+        <v>116.085914379844</v>
+      </c>
+      <c r="W29" s="3">
+        <v>10</v>
+      </c>
+      <c r="X29" s="3">
+        <v>106.076436473556</v>
+      </c>
+      <c r="Y29" s="3">
+        <f t="shared" si="30"/>
+        <v>3.6046705173587239</v>
+      </c>
+      <c r="Z29" s="3">
+        <f t="shared" si="31"/>
+        <v>382.37060314270292</v>
+      </c>
+      <c r="AA29" s="3">
+        <v>46.962113624420603</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>45208</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>143.02392510125</v>
+      </c>
+      <c r="AD29" s="3">
+        <f t="shared" si="32"/>
+        <v>4.1112423051113485</v>
+      </c>
+      <c r="AE29" s="3">
+        <f t="shared" si="33"/>
+        <v>588.00601151933586</v>
+      </c>
+      <c r="AF29" s="3">
+        <v>240.00057640028601</v>
+      </c>
+      <c r="AG29" s="3">
+        <v>116.085914379844</v>
+      </c>
+      <c r="AH29" s="3">
+        <v>20</v>
+      </c>
+      <c r="AI29" s="3">
+        <v>96.066686484846301</v>
+      </c>
+      <c r="AJ29" s="3">
+        <f t="shared" si="34"/>
+        <v>3.4508436746530169</v>
+      </c>
+      <c r="AK29" s="3">
+        <f t="shared" si="35"/>
+        <v>331.51111740110633</v>
+      </c>
+      <c r="AL29" s="3">
+        <v>46.962113624420603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>